<commit_message>
add content EclaireStudyPhaseCS 737d3a52f977e9c3ac207ea0e9446902235f60b8
</commit_message>
<xml_diff>
--- a/ig/sd-correction-conceptmaps/CodeSystem-eclaire-study-phase-code-system.xlsx
+++ b/ig/sd-correction-conceptmaps/CodeSystem-eclaire-study-phase-code-system.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-01T16:27:26+00:00</t>
+    <t>2023-09-01T17:43:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -105,28 +105,31 @@
     <t>Content</t>
   </si>
   <si>
-    <t>complete</t>
+    <t>supplement</t>
   </si>
   <si>
     <t>Supplements</t>
   </si>
   <si>
+    <t>http://terminology.hl7.org/CodeSystem/research-study-phase</t>
+  </si>
+  <si>
     <t>Count</t>
   </si>
   <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>Definition</t>
   </si>
   <si>
     <t>phase-3-phase-4</t>
@@ -421,15 +424,15 @@
       <c r="A20" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" t="s" s="2">
+        <v>32</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s" s="2">
         <v>33</v>
       </c>
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -460,16 +463,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add content complete c59788d65d19d4393499410816bd173ef1bbee6e
</commit_message>
<xml_diff>
--- a/ig/sd-correction-conceptmaps/CodeSystem-eclaire-study-phase-code-system.xlsx
+++ b/ig/sd-correction-conceptmaps/CodeSystem-eclaire-study-phase-code-system.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-01T17:52:23+00:00</t>
+    <t>2023-09-01T18:07:06+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -105,7 +105,7 @@
     <t>Content</t>
   </si>
   <si>
-    <t>supplement</t>
+    <t>complete</t>
   </si>
   <si>
     <t>Supplements</t>
@@ -117,6 +117,9 @@
     <t>Count</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Level</t>
   </si>
   <si>
@@ -127,9 +130,6 @@
   </si>
   <si>
     <t>Definition</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>phase-3-phase-4</t>
@@ -432,7 +432,9 @@
       <c r="A21" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" t="s" s="2">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -449,21 +451,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="2">
         <v>39</v>

</xml_diff>